<commit_message>
Alteracao na tabela aluno Criacao de novas tabelas (endereco e endereco_aluno)
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Informatica\Documents\NetBeansProjects\fenix\fenixschool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Informatica\Documents\GitHub\fenixschool\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,9 +53,6 @@
     <t>04 a 12 de Agosto</t>
   </si>
   <si>
-    <t>CRUD - Candidato</t>
-  </si>
-  <si>
     <t>CRUD - Funcionario</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>04 a 18 de Setembro</t>
+  </si>
+  <si>
+    <t>CRUD - Candidato, Artigo, CategoriaArtigo</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -460,10 +460,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -471,27 +471,27 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,13 +499,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,13 +513,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,13 +527,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,10 +541,10 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,10 +552,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>